<commit_message>
Entregable 2 y 3
</commit_message>
<xml_diff>
--- a/src/Excel/entregable1/AltaCuentaAhorro.xlsx
+++ b/src/Excel/entregable1/AltaCuentaAhorro.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DEA11A-91BE-4FCE-BD9C-9AE738BA041D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A1B365-1EA2-4D17-B1DC-0054C0F57C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AltaCuentaAhorro" sheetId="5" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Usuario</t>
   </si>
@@ -35,9 +35,6 @@
     <t>123456</t>
   </si>
   <si>
-    <t>4793147</t>
-  </si>
-  <si>
     <t>100005</t>
   </si>
   <si>
@@ -50,20 +47,17 @@
     <t>Transaccion</t>
   </si>
   <si>
-    <t>PASSED</t>
-  </si>
-  <si>
-    <t>AAACT23066XNW7Z87</t>
-  </si>
-  <si>
-    <t>7 mar. 2023, 10:06:06</t>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>4793400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +69,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A91A77-E5B6-4AE4-A13D-A81F28ECF0AB}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,12 +482,12 @@
     <col min="1" max="1" width="12.08984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="4" width="10.90625" style="1" collapsed="1"/>
     <col min="5" max="5" width="12.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="18.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="10.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -501,16 +501,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -518,22 +521,17 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PASSED">
       <formula>NOT(ISERROR(SEARCH("PASSED",A1)))</formula>

</xml_diff>

<commit_message>
update alta cuenta ahorro
</commit_message>
<xml_diff>
--- a/src/Excel/entregable1/AltaCuentaAhorro.xlsx
+++ b/src/Excel/entregable1/AltaCuentaAhorro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295D4451-28A2-4CF2-B1D3-D7D03368F15F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3FB2F9-7BB1-4FA9-85DD-A08B990A78A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,9 +29,6 @@
     <t>ejecutivo</t>
   </si>
   <si>
-    <t>SCISNEROSA1</t>
-  </si>
-  <si>
     <t>123456</t>
   </si>
   <si>
@@ -50,16 +47,19 @@
     <t>Cuenta</t>
   </si>
   <si>
-    <t>4793400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAACT23139LF2RZNVC </t>
-  </si>
-  <si>
-    <t>19 may. 2023, 11:11:00</t>
-  </si>
-  <si>
     <t>PASSED</t>
+  </si>
+  <si>
+    <t>dmoralesr</t>
+  </si>
+  <si>
+    <t>2103764</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAACT231729MLH238M </t>
+  </si>
+  <si>
+    <t>21 jun. 2023, 14:50:44</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -511,42 +511,42 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2">
-        <v>1010802788</v>
+        <v>1010824482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update entregable 1, 2 y 3
</commit_message>
<xml_diff>
--- a/src/Excel/entregable1/AltaCuentaAhorro.xlsx
+++ b/src/Excel/entregable1/AltaCuentaAhorro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7284A5B-9B20-4F70-B5A3-9BC8B19CFEE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A2475C-D76F-4A6B-AE56-FB1C0B299312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Usuario</t>
   </si>
@@ -44,22 +44,37 @@
     <t>Cuenta</t>
   </si>
   <si>
+    <t>dmoralesr</t>
+  </si>
+  <si>
+    <t>2103764</t>
+  </si>
+  <si>
+    <t>CodCliente</t>
+  </si>
+  <si>
+    <t>cuenta</t>
+  </si>
+  <si>
+    <t>Cuenta Simple</t>
+  </si>
+  <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>dmoralesr</t>
-  </si>
-  <si>
-    <t>2103764</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAACT231729MLH238M </t>
-  </si>
-  <si>
-    <t>21 jun. 2023, 14:50:44</t>
-  </si>
-  <si>
-    <t>CodCliente</t>
+    <t>1010826248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAACT231810953MV37 </t>
+  </si>
+  <si>
+    <t>30 jun. 2023, 14:07:30</t>
+  </si>
+  <si>
+    <t>moneda</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -480,24 +495,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A91A77-E5B6-4AE4-A13D-A81F28ECF0AB}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="4" width="10.90625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.90625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="10.90625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.90625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="10.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -505,48 +521,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>1010824482</v>
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update entregable 1, 2
</commit_message>
<xml_diff>
--- a/src/Excel/entregable1/AltaCuentaAhorro.xlsx
+++ b/src/Excel/entregable1/AltaCuentaAhorro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A2475C-D76F-4A6B-AE56-FB1C0B299312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EB7241-161E-4252-9FE8-51FB4D0D642B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>CodCliente</t>
   </si>
   <si>
-    <t>cuenta</t>
-  </si>
-  <si>
     <t>Cuenta Simple</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Tipo de Producto</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +506,8 @@
     <col min="1" max="1" width="12.08984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="4" width="10.90625" style="1" collapsed="1"/>
     <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="20.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="19.90625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
@@ -527,10 +528,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
@@ -559,22 +560,22 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>